<commit_message>
Função de export atualizada
</commit_message>
<xml_diff>
--- a/projetoana/ListaKernels.xlsx
+++ b/projetoana/ListaKernels.xlsx
@@ -175,6 +175,20 @@
         <v>3.0</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
     <row r="5">
       <c r="A5" t="n">
         <v>0.0</v>
@@ -270,20 +284,6 @@
         <v>0.0</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="B12" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D12" t="n">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Iniciando a interface do usuário.
</commit_message>
<xml_diff>
--- a/projetoana/ListaKernels.xlsx
+++ b/projetoana/ListaKernels.xlsx
@@ -66,562 +66,562 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-0.08667836338281631</v>
+        <v>-0.03645937889814377</v>
       </c>
       <c r="B1" t="n">
-        <v>0.15919843316078186</v>
+        <v>-0.02489970624446869</v>
       </c>
       <c r="C1" t="n">
-        <v>-0.08567188680171967</v>
+        <v>0.20854738354682922</v>
       </c>
       <c r="D1" t="n">
-        <v>0.30606794357299805</v>
+        <v>0.09746034443378448</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.0607571005821228</v>
+        <v>0.040239233523607254</v>
       </c>
       <c r="B2" t="n">
-        <v>0.08930443227291107</v>
+        <v>0.1388837993144989</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0915321484208107</v>
+        <v>0.08274422585964203</v>
       </c>
       <c r="D2" t="n">
-        <v>0.006435009650886059</v>
+        <v>0.08232927322387695</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-0.14793811738491058</v>
+        <v>0.13825607299804688</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.21708253026008606</v>
+        <v>-0.11552521586418152</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.005357176065444946</v>
+        <v>-0.03248145431280136</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.3578645586967468</v>
+        <v>-0.15499602258205414</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.025178100913763046</v>
+        <v>0.003860547672957182</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.05453399196267128</v>
+        <v>-0.038160040974617004</v>
       </c>
       <c r="C4" t="n">
-        <v>0.14015652239322662</v>
+        <v>-0.04856916889548302</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.02475045993924141</v>
+        <v>0.006127014756202698</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.03634659945964813</v>
+        <v>-0.05571295693516731</v>
       </c>
       <c r="B5" t="n">
-        <v>0.11412395536899567</v>
+        <v>0.08726853132247925</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.06431213021278381</v>
+        <v>-0.12013419717550278</v>
       </c>
       <c r="D5" t="n">
-        <v>0.18697920441627502</v>
+        <v>-0.07477033138275146</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.06445445865392685</v>
+        <v>0.03239799290895462</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.009638765826821327</v>
+        <v>0.055462416261434555</v>
       </c>
       <c r="C6" t="n">
-        <v>0.15087860822677612</v>
+        <v>-0.03682498633861542</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0855238288640976</v>
+        <v>0.02580605447292328</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-0.1555798053741455</v>
+        <v>0.11995808780193329</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.04941423982381821</v>
+        <v>-0.006937410682439804</v>
       </c>
       <c r="C7" t="n">
-        <v>0.11428406834602356</v>
+        <v>0.029618196189403534</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.012793129310011864</v>
+        <v>-0.005316995549947023</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-0.20398259162902832</v>
+        <v>-0.31964772939682007</v>
       </c>
       <c r="B8" t="n">
-        <v>0.1368585228919983</v>
+        <v>-0.12309758365154266</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1450652778148651</v>
+        <v>0.16752608120441437</v>
       </c>
       <c r="D8" t="n">
-        <v>0.20196694135665894</v>
+        <v>0.031491782516241074</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.09085401147603989</v>
+        <v>0.07639074325561523</v>
       </c>
       <c r="B9" t="n">
-        <v>0.04444570094347</v>
+        <v>-0.007258182391524315</v>
       </c>
       <c r="C9" t="n">
-        <v>0.11406052112579346</v>
+        <v>-0.07923941314220428</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.029377531260252</v>
+        <v>0.08470811694860458</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-0.17525893449783325</v>
+        <v>0.007324728183448315</v>
       </c>
       <c r="B10" t="n">
-        <v>0.025939326733350754</v>
+        <v>0.04319918155670166</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.20776057243347168</v>
+        <v>0.12437185645103455</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.09797161817550659</v>
+        <v>-0.016205724328756332</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>-0.09909474849700928</v>
+        <v>0.03911978378891945</v>
       </c>
       <c r="B11" t="n">
-        <v>0.07868676632642746</v>
+        <v>-0.04634231701493263</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.22764916718006134</v>
+        <v>-0.013060078024864197</v>
       </c>
       <c r="D11" t="n">
-        <v>0.15831045806407928</v>
+        <v>-0.13691674172878265</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>-0.08072030544281006</v>
+        <v>-0.09196224808692932</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.1389293521642685</v>
+        <v>-0.0021154657006263733</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.09345214068889618</v>
+        <v>0.156947523355484</v>
       </c>
       <c r="D12" t="n">
-        <v>0.015877477824687958</v>
+        <v>0.03901771456003189</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>-0.049545902758836746</v>
+        <v>-0.07150474935770035</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.10803447663784027</v>
+        <v>0.10515344142913818</v>
       </c>
       <c r="C13" t="n">
-        <v>0.02453118935227394</v>
+        <v>-0.04622673988342285</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.10604232549667358</v>
+        <v>0.06997884064912796</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.05489186570048332</v>
+        <v>0.04358452558517456</v>
       </c>
       <c r="B14" t="n">
-        <v>0.09273608028888702</v>
+        <v>-0.1785842329263687</v>
       </c>
       <c r="C14" t="n">
-        <v>0.05301080271601677</v>
+        <v>-0.03553538769483566</v>
       </c>
       <c r="D14" t="n">
-        <v>0.004195998422801495</v>
+        <v>0.033925995230674744</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>-0.053909387439489365</v>
+        <v>0.030419476330280304</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.1711776852607727</v>
+        <v>0.022231802344322205</v>
       </c>
       <c r="C15" t="n">
-        <v>0.029295651242136955</v>
+        <v>-0.034319594502449036</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.09874629974365234</v>
+        <v>-0.01827199198305607</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.009096547961235046</v>
+        <v>0.10198475420475006</v>
       </c>
       <c r="B16" t="n">
-        <v>0.07634221762418747</v>
+        <v>0.017157435417175293</v>
       </c>
       <c r="C16" t="n">
-        <v>0.008414281532168388</v>
+        <v>-0.015963619574904442</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.013739289715886116</v>
+        <v>0.1405799686908722</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.07066864520311356</v>
+        <v>-0.05079837143421173</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.10637517273426056</v>
+        <v>-0.055032096803188324</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.043973665684461594</v>
+        <v>1.5768781304359436E-4</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0829370766878128</v>
+        <v>-0.212811678647995</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>-0.007018933072686195</v>
+        <v>0.009564101696014404</v>
       </c>
       <c r="B18" t="n">
-        <v>0.07369450479745865</v>
+        <v>0.024477137252688408</v>
       </c>
       <c r="C18" t="n">
-        <v>0.13900642096996307</v>
+        <v>-0.07099685072898865</v>
       </c>
       <c r="D18" t="n">
-        <v>0.05617520585656166</v>
+        <v>-0.013599954545497894</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>-0.16725888848304749</v>
+        <v>0.10725601017475128</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.10125395655632019</v>
+        <v>-0.16258364915847778</v>
       </c>
       <c r="C19" t="n">
-        <v>0.030373696237802505</v>
+        <v>0.06872893869876862</v>
       </c>
       <c r="D19" t="n">
-        <v>0.08055175840854645</v>
+        <v>-0.00268564373254776</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>-0.2894055247306824</v>
+        <v>0.03698643669486046</v>
       </c>
       <c r="B20" t="n">
-        <v>0.06996780633926392</v>
+        <v>-0.004362802952528</v>
       </c>
       <c r="C20" t="n">
-        <v>0.030088156461715698</v>
+        <v>0.1236998438835144</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.05262046307325363</v>
+        <v>-0.04996020719408989</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.015983253717422485</v>
+        <v>-0.05389824137091637</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.0549190454185009</v>
+        <v>-0.09831301122903824</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.21299506723880768</v>
+        <v>-0.10829125344753265</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.17180350422859192</v>
+        <v>0.06925938278436661</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>-0.038383401930332184</v>
+        <v>-0.05727848783135414</v>
       </c>
       <c r="B22" t="n">
-        <v>0.086825430393219</v>
+        <v>0.17100811004638672</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.07372735440731049</v>
+        <v>-0.2096560001373291</v>
       </c>
       <c r="D22" t="n">
-        <v>-0.07293318212032318</v>
+        <v>-0.08324433118104935</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>-0.22583052515983582</v>
+        <v>-0.0639127641916275</v>
       </c>
       <c r="B23" t="n">
-        <v>0.265401691198349</v>
+        <v>0.01711965724825859</v>
       </c>
       <c r="C23" t="n">
-        <v>0.006137438118457794</v>
+        <v>0.2780313193798065</v>
       </c>
       <c r="D23" t="n">
-        <v>-0.008326712064445019</v>
+        <v>0.16129446029663086</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.04068708419799805</v>
+        <v>0.0806933045387268</v>
       </c>
       <c r="B24" t="n">
-        <v>0.005329933017492294</v>
+        <v>0.1447765976190567</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.12982967495918274</v>
+        <v>0.017224323004484177</v>
       </c>
       <c r="D24" t="n">
-        <v>0.19694453477859497</v>
+        <v>-0.06272125244140625</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.021221499890089035</v>
+        <v>0.04145818203687668</v>
       </c>
       <c r="B25" t="n">
-        <v>0.042629972100257874</v>
+        <v>0.031215110793709755</v>
       </c>
       <c r="C25" t="n">
-        <v>0.0010616183280944824</v>
+        <v>0.01554529182612896</v>
       </c>
       <c r="D25" t="n">
-        <v>0.19442281126976013</v>
+        <v>0.007098853588104248</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>-0.04027947038412094</v>
+        <v>-0.02616555243730545</v>
       </c>
       <c r="B26" t="n">
-        <v>0.2536635398864746</v>
+        <v>-0.03469093143939972</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.1398487091064453</v>
+        <v>-0.1359042376279831</v>
       </c>
       <c r="D26" t="n">
-        <v>0.017916642129421234</v>
+        <v>-0.003923187963664532</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.010023482143878937</v>
+        <v>-0.02605546824634075</v>
       </c>
       <c r="B27" t="n">
-        <v>-0.06880146265029907</v>
+        <v>-0.16140492260456085</v>
       </c>
       <c r="C27" t="n">
-        <v>0.01259925588965416</v>
+        <v>-0.06940178573131561</v>
       </c>
       <c r="D27" t="n">
-        <v>0.029710261151194572</v>
+        <v>0.04508860781788826</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>-0.24337893724441528</v>
+        <v>-0.12115830183029175</v>
       </c>
       <c r="B28" t="n">
-        <v>-0.04626532644033432</v>
+        <v>-0.00753848347812891</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.22665099799633026</v>
+        <v>-0.21343901753425598</v>
       </c>
       <c r="D28" t="n">
-        <v>0.00597245991230011</v>
+        <v>0.002133619971573353</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>-0.012028882279992104</v>
+        <v>0.04842618107795715</v>
       </c>
       <c r="B29" t="n">
-        <v>-0.08752290159463882</v>
+        <v>0.10341055691242218</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.0203273706138134</v>
+        <v>0.04518997296690941</v>
       </c>
       <c r="D29" t="n">
-        <v>-0.055110663175582886</v>
+        <v>-0.1666748821735382</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.23698744177818298</v>
+        <v>0.009728776291012764</v>
       </c>
       <c r="B30" t="n">
-        <v>-0.06799624860286713</v>
+        <v>-0.14674586057662964</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.15639202296733856</v>
+        <v>-0.03645876422524452</v>
       </c>
       <c r="D30" t="n">
-        <v>0.024382155388593674</v>
+        <v>0.006158744916319847</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>-0.07815629243850708</v>
+        <v>-0.011175533756613731</v>
       </c>
       <c r="B31" t="n">
-        <v>0.12586922943592072</v>
+        <v>0.09510790556669235</v>
       </c>
       <c r="C31" t="n">
-        <v>0.024115052074193954</v>
+        <v>0.11795547604560852</v>
       </c>
       <c r="D31" t="n">
-        <v>0.08285757899284363</v>
+        <v>0.036981526762247086</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>-0.1346912682056427</v>
+        <v>-0.2249990701675415</v>
       </c>
       <c r="B32" t="n">
-        <v>-0.004279911518096924</v>
+        <v>0.14667731523513794</v>
       </c>
       <c r="C32" t="n">
-        <v>2.5521236239001155E-4</v>
+        <v>0.039843350648880005</v>
       </c>
       <c r="D32" t="n">
-        <v>-0.045220453292131424</v>
+        <v>-0.012270011007785797</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>-0.021350374445319176</v>
+        <v>0.07825946807861328</v>
       </c>
       <c r="B33" t="n">
-        <v>0.16700045764446259</v>
+        <v>0.08022639155387878</v>
       </c>
       <c r="C33" t="n">
-        <v>0.01964055374264717</v>
+        <v>-0.006772227585315704</v>
       </c>
       <c r="D33" t="n">
-        <v>0.03975813463330269</v>
+        <v>0.10474631190299988</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>-0.011913873255252838</v>
+        <v>-0.023772763088345528</v>
       </c>
       <c r="B34" t="n">
-        <v>0.03418285772204399</v>
+        <v>-0.07644307613372803</v>
       </c>
       <c r="C34" t="n">
-        <v>0.08175808191299438</v>
+        <v>-6.343461573123932E-4</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.05529468134045601</v>
+        <v>0.08040252327919006</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0.046362318098545074</v>
+        <v>-0.04601811245083809</v>
       </c>
       <c r="B35" t="n">
-        <v>-0.055842697620391846</v>
+        <v>-0.009052349254488945</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.013910874724388123</v>
+        <v>0.0762367993593216</v>
       </c>
       <c r="D35" t="n">
-        <v>0.0802222266793251</v>
+        <v>-0.0630655437707901</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>-0.0336122065782547</v>
+        <v>-0.03716910257935524</v>
       </c>
       <c r="B36" t="n">
-        <v>0.21987532079219818</v>
+        <v>0.08829278498888016</v>
       </c>
       <c r="C36" t="n">
-        <v>-0.07161958515644073</v>
+        <v>0.054020702838897705</v>
       </c>
       <c r="D36" t="n">
-        <v>-0.19364652037620544</v>
+        <v>0.012886494398117065</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>-0.07454369962215424</v>
+        <v>0.002858886495232582</v>
       </c>
       <c r="B37" t="n">
-        <v>0.22222179174423218</v>
+        <v>-0.2365773767232895</v>
       </c>
       <c r="C37" t="n">
-        <v>-0.16759255528450012</v>
+        <v>0.015892114490270615</v>
       </c>
       <c r="D37" t="n">
-        <v>0.03167300298810005</v>
+        <v>4.676170647144318E-6</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0.03344985842704773</v>
+        <v>-0.04663930833339691</v>
       </c>
       <c r="B38" t="n">
-        <v>0.10406787693500519</v>
+        <v>-0.025227811187505722</v>
       </c>
       <c r="C38" t="n">
-        <v>0.19035997986793518</v>
+        <v>0.0377935953438282</v>
       </c>
       <c r="D38" t="n">
-        <v>-0.07494823634624481</v>
+        <v>-0.0017309768591076136</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0.06775104999542236</v>
+        <v>0.047560855746269226</v>
       </c>
       <c r="B39" t="n">
-        <v>-0.008994216099381447</v>
+        <v>-0.23718826472759247</v>
       </c>
       <c r="C39" t="n">
-        <v>0.0736740455031395</v>
+        <v>-0.050094474107027054</v>
       </c>
       <c r="D39" t="n">
-        <v>0.0749136358499527</v>
+        <v>-0.06706572324037552</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0.03477755934000015</v>
+        <v>-0.020689867436885834</v>
       </c>
       <c r="B40" t="n">
-        <v>-0.014132904820144176</v>
+        <v>-0.004362897947430611</v>
       </c>
       <c r="C40" t="n">
-        <v>0.07370069622993469</v>
+        <v>0.01911557838320732</v>
       </c>
       <c r="D40" t="n">
-        <v>0.03893888369202614</v>
+        <v>-0.05207189917564392</v>
       </c>
     </row>
   </sheetData>
@@ -639,562 +639,562 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-0.10686135292053223</v>
+        <v>0.008354302495718002</v>
       </c>
       <c r="B1" t="n">
-        <v>0.16547265648841858</v>
+        <v>0.05542655289173126</v>
       </c>
       <c r="C1" t="n">
-        <v>0.16051197052001953</v>
+        <v>-0.07463593035936356</v>
       </c>
       <c r="D1" t="n">
-        <v>0.04651203379034996</v>
+        <v>-0.020648127421736717</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.26431936025619507</v>
+        <v>0.08855143934488297</v>
       </c>
       <c r="B2" t="n">
-        <v>0.006028580479323864</v>
+        <v>0.0349276065826416</v>
       </c>
       <c r="C2" t="n">
-        <v>0.007579152937978506</v>
+        <v>0.00854293629527092</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.0707450807094574</v>
+        <v>-0.048725537955760956</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-0.09422853589057922</v>
+        <v>0.1385767161846161</v>
       </c>
       <c r="B3" t="n">
-        <v>0.1801951825618744</v>
+        <v>-0.19232559204101562</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.13453945517539978</v>
+        <v>0.046580418944358826</v>
       </c>
       <c r="D3" t="n">
-        <v>0.05195818841457367</v>
+        <v>-0.07082438468933105</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.1243370845913887</v>
+        <v>0.05728478729724884</v>
       </c>
       <c r="B4" t="n">
-        <v>0.10433927178382874</v>
+        <v>0.012976162135601044</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.010545622557401657</v>
+        <v>0.014187956228852272</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.2790784239768982</v>
+        <v>0.0889013484120369</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-0.17101731896400452</v>
+        <v>0.24765315651893616</v>
       </c>
       <c r="B5" t="n">
-        <v>0.026578012853860855</v>
+        <v>-0.056981489062309265</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.03017488680779934</v>
+        <v>-6.038863211870193E-4</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.14940449595451355</v>
+        <v>-0.23722219467163086</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.08764567971229553</v>
+        <v>0.1376321166753769</v>
       </c>
       <c r="B6" t="n">
-        <v>0.005514027550816536</v>
+        <v>-0.07498213648796082</v>
       </c>
       <c r="C6" t="n">
-        <v>0.16060735285282135</v>
+        <v>0.08970347791910172</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.08388200402259827</v>
+        <v>-0.09653335809707642</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.015915796160697937</v>
+        <v>-0.12228547781705856</v>
       </c>
       <c r="B7" t="n">
-        <v>0.36513492465019226</v>
+        <v>-0.11624995619058609</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.007519811391830444</v>
+        <v>0.09236159175634384</v>
       </c>
       <c r="D7" t="n">
-        <v>0.24847543239593506</v>
+        <v>-0.08209969848394394</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.06022512912750244</v>
+        <v>0.03363914042711258</v>
       </c>
       <c r="B8" t="n">
-        <v>0.08602756261825562</v>
+        <v>-0.007285371422767639</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.02594143897294998</v>
+        <v>0.1063380092382431</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.056686773896217346</v>
+        <v>-0.021463245153427124</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-0.04705369845032692</v>
+        <v>0.05868157371878624</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.09665875136852264</v>
+        <v>0.0836232602596283</v>
       </c>
       <c r="C9" t="n">
-        <v>0.03301076591014862</v>
+        <v>-0.052407633513212204</v>
       </c>
       <c r="D9" t="n">
-        <v>0.05700724571943283</v>
+        <v>0.0013695023953914642</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.26302576065063477</v>
+        <v>0.005955059081315994</v>
       </c>
       <c r="B10" t="n">
-        <v>0.015838056802749634</v>
+        <v>-0.14469368755817413</v>
       </c>
       <c r="C10" t="n">
-        <v>0.14171116054058075</v>
+        <v>-0.13315200805664062</v>
       </c>
       <c r="D10" t="n">
-        <v>0.09518961608409882</v>
+        <v>0.06232134997844696</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>-0.11731787770986557</v>
+        <v>-0.21400848031044006</v>
       </c>
       <c r="B11" t="n">
-        <v>0.05561298877000809</v>
+        <v>0.03603436052799225</v>
       </c>
       <c r="C11" t="n">
-        <v>0.04275549203157425</v>
+        <v>-0.06539740413427353</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.027257945388555527</v>
+        <v>0.034728992730379105</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.004822995513677597</v>
+        <v>0.019194290041923523</v>
       </c>
       <c r="B12" t="n">
-        <v>0.06269501149654388</v>
+        <v>-0.013569889590144157</v>
       </c>
       <c r="C12" t="n">
-        <v>0.07657235860824585</v>
+        <v>-0.059904225170612335</v>
       </c>
       <c r="D12" t="n">
-        <v>0.015301588922739029</v>
+        <v>0.1390058994293213</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.04495428130030632</v>
+        <v>0.008117038756608963</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.05532301962375641</v>
+        <v>0.018306508660316467</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.2432018518447876</v>
+        <v>-0.04216401278972626</v>
       </c>
       <c r="D13" t="n">
-        <v>0.023858480155467987</v>
+        <v>0.01915864646434784</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>-0.12047471106052399</v>
+        <v>0.007521694526076317</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.059923868626356125</v>
+        <v>0.0015739863738417625</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.028042547404766083</v>
+        <v>0.03745278716087341</v>
       </c>
       <c r="D14" t="n">
-        <v>0.08219468593597412</v>
+        <v>0.009523640386760235</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>-0.06171991676092148</v>
+        <v>0.04238365590572357</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.10009010136127472</v>
+        <v>-0.03340046480298042</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.08360809832811356</v>
+        <v>-0.034096021205186844</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0019305003806948662</v>
+        <v>-0.04386261850595474</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.2089879810810089</v>
+        <v>0.002814288716763258</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.0410563126206398</v>
+        <v>0.05611598491668701</v>
       </c>
       <c r="C16" t="n">
-        <v>0.023873653262853622</v>
+        <v>-0.022056493908166885</v>
       </c>
       <c r="D16" t="n">
-        <v>0.16237595677375793</v>
+        <v>-0.12594950199127197</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>-0.16713523864746094</v>
+        <v>0.06403426826000214</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.010772336274385452</v>
+        <v>-0.05824148654937744</v>
       </c>
       <c r="C17" t="n">
-        <v>0.03538428246974945</v>
+        <v>-0.03979247435927391</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.2422255575656891</v>
+        <v>0.1501792073249817</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.019552722573280334</v>
+        <v>0.08928427845239639</v>
       </c>
       <c r="B18" t="n">
-        <v>0.03821398690342903</v>
+        <v>0.052875056862831116</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.0054355189204216</v>
+        <v>0.06306224316358566</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.02586422488093376</v>
+        <v>0.0749635323882103</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>-0.0335141122341156</v>
+        <v>0.01277395710349083</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.0546705424785614</v>
+        <v>-0.002139367163181305</v>
       </c>
       <c r="C19" t="n">
-        <v>0.2725825309753418</v>
+        <v>0.07237928360700607</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.059554822742938995</v>
+        <v>-0.04089367017149925</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>-0.0645197257399559</v>
+        <v>0.019388560205698013</v>
       </c>
       <c r="B20" t="n">
-        <v>0.0406014621257782</v>
+        <v>0.09321679919958115</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.027524515986442566</v>
+        <v>-0.02800765633583069</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.16345065832138062</v>
+        <v>-0.07503608614206314</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.09202352911233902</v>
+        <v>-0.05283130705356598</v>
       </c>
       <c r="B21" t="n">
-        <v>0.10082858800888062</v>
+        <v>0.012143619358539581</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.05084315687417984</v>
+        <v>0.025037838146090508</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.08373826742172241</v>
+        <v>-0.03760942071676254</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.02312145009636879</v>
+        <v>0.008673112839460373</v>
       </c>
       <c r="B22" t="n">
-        <v>0.0012169703841209412</v>
+        <v>0.10663142055273056</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.15494203567504883</v>
+        <v>-0.19375386834144592</v>
       </c>
       <c r="D22" t="n">
-        <v>0.013545813038945198</v>
+        <v>-0.022504761815071106</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.11849303543567657</v>
+        <v>0.08615938574075699</v>
       </c>
       <c r="B23" t="n">
-        <v>0.03339091315865517</v>
+        <v>-0.04631542041897774</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.01669771410524845</v>
+        <v>-0.03778215870261192</v>
       </c>
       <c r="D23" t="n">
-        <v>-0.08717069029808044</v>
+        <v>0.014504976570606232</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>-0.03081430494785309</v>
+        <v>0.12417358160018921</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.010042843408882618</v>
+        <v>0.02204757183790207</v>
       </c>
       <c r="C24" t="n">
-        <v>0.2248476892709732</v>
+        <v>0.03296434134244919</v>
       </c>
       <c r="D24" t="n">
-        <v>0.0886191725730896</v>
+        <v>0.004541794769465923</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.19385366141796112</v>
+        <v>0.1120496466755867</v>
       </c>
       <c r="B25" t="n">
-        <v>0.013064437545835972</v>
+        <v>-0.08078446984291077</v>
       </c>
       <c r="C25" t="n">
-        <v>0.1644504815340042</v>
+        <v>-0.08755286037921906</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.001775447279214859</v>
+        <v>-0.02508552372455597</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.0784287303686142</v>
+        <v>0.052187636494636536</v>
       </c>
       <c r="B26" t="n">
-        <v>0.03797762840986252</v>
+        <v>-0.033438827842473984</v>
       </c>
       <c r="C26" t="n">
-        <v>0.05786563828587532</v>
+        <v>-0.03299400210380554</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.10396172851324081</v>
+        <v>-0.002921540290117264</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>-2.4494994431734085E-4</v>
+        <v>-0.18928231298923492</v>
       </c>
       <c r="B27" t="n">
-        <v>0.18226808309555054</v>
+        <v>0.012691829353570938</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.13697929680347443</v>
+        <v>0.021157607436180115</v>
       </c>
       <c r="D27" t="n">
-        <v>0.12479393184185028</v>
+        <v>-0.1927630603313446</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>-0.05091041699051857</v>
+        <v>0.09522995352745056</v>
       </c>
       <c r="B28" t="n">
-        <v>-0.07325101643800735</v>
+        <v>-0.08103126287460327</v>
       </c>
       <c r="C28" t="n">
-        <v>0.08223508298397064</v>
+        <v>0.005646871402859688</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.04354014992713928</v>
+        <v>0.06777035444974899</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0.049251023679971695</v>
+        <v>-0.1340988576412201</v>
       </c>
       <c r="B29" t="n">
-        <v>-0.17480799555778503</v>
+        <v>-0.15134964883327484</v>
       </c>
       <c r="C29" t="n">
-        <v>0.05047837644815445</v>
+        <v>-0.05027034878730774</v>
       </c>
       <c r="D29" t="n">
-        <v>0.12272758781909943</v>
+        <v>0.09816094487905502</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>-0.04270625859498978</v>
+        <v>-0.06391935050487518</v>
       </c>
       <c r="B30" t="n">
-        <v>-0.2041558027267456</v>
+        <v>0.06877727806568146</v>
       </c>
       <c r="C30" t="n">
-        <v>0.11360684037208557</v>
+        <v>0.03285427391529083</v>
       </c>
       <c r="D30" t="n">
-        <v>0.02803165279328823</v>
+        <v>0.1596432626247406</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>-0.19568414986133575</v>
+        <v>0.3874761760234833</v>
       </c>
       <c r="B31" t="n">
-        <v>0.04908212274312973</v>
+        <v>0.08722516894340515</v>
       </c>
       <c r="C31" t="n">
-        <v>-0.010813005268573761</v>
+        <v>0.06339703500270844</v>
       </c>
       <c r="D31" t="n">
-        <v>-0.027524597942829132</v>
+        <v>0.06014786288142204</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.07394783198833466</v>
+        <v>-0.001097165048122406</v>
       </c>
       <c r="B32" t="n">
-        <v>-0.05361825227737427</v>
+        <v>0.013132515363395214</v>
       </c>
       <c r="C32" t="n">
-        <v>-0.06551547348499298</v>
+        <v>-0.06257474422454834</v>
       </c>
       <c r="D32" t="n">
-        <v>0.01594138890504837</v>
+        <v>-0.14151421189308167</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>-0.04832921922206879</v>
+        <v>-0.009396892972290516</v>
       </c>
       <c r="B33" t="n">
-        <v>0.21604663133621216</v>
+        <v>-0.05863890051841736</v>
       </c>
       <c r="C33" t="n">
-        <v>0.045328084379434586</v>
+        <v>-0.05136873200535774</v>
       </c>
       <c r="D33" t="n">
-        <v>-0.07039772719144821</v>
+        <v>-0.14193204045295715</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>-0.04153161123394966</v>
+        <v>-0.09131227433681488</v>
       </c>
       <c r="B34" t="n">
-        <v>-0.035734549164772034</v>
+        <v>0.0319991298019886</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.11665034294128418</v>
+        <v>-0.014334521256387234</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.0434885136783123</v>
+        <v>0.1777394413948059</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>-0.03610339015722275</v>
+        <v>0.04383425414562225</v>
       </c>
       <c r="B35" t="n">
-        <v>-0.018783627077937126</v>
+        <v>0.07319198548793793</v>
       </c>
       <c r="C35" t="n">
-        <v>0.006789013743400574</v>
+        <v>0.06098277121782303</v>
       </c>
       <c r="D35" t="n">
-        <v>-0.054787371307611465</v>
+        <v>0.012368150055408478</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0.09279844164848328</v>
+        <v>-0.008837684988975525</v>
       </c>
       <c r="B36" t="n">
-        <v>-0.06442714482545853</v>
+        <v>-0.154570072889328</v>
       </c>
       <c r="C36" t="n">
-        <v>0.10623171180486679</v>
+        <v>-0.04405355453491211</v>
       </c>
       <c r="D36" t="n">
-        <v>0.07153469324111938</v>
+        <v>-0.012575069442391396</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0.016476914286613464</v>
+        <v>-0.04649978131055832</v>
       </c>
       <c r="B37" t="n">
-        <v>0.1441464126110077</v>
+        <v>0.19604608416557312</v>
       </c>
       <c r="C37" t="n">
-        <v>-0.06826889514923096</v>
+        <v>-0.14556381106376648</v>
       </c>
       <c r="D37" t="n">
-        <v>-0.07676643133163452</v>
+        <v>-0.004110058769583702</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0.011275600641965866</v>
+        <v>0.18963637948036194</v>
       </c>
       <c r="B38" t="n">
-        <v>0.05724171921610832</v>
+        <v>0.2178233116865158</v>
       </c>
       <c r="C38" t="n">
-        <v>-0.038269590586423874</v>
+        <v>-0.07431188225746155</v>
       </c>
       <c r="D38" t="n">
-        <v>0.011661751195788383</v>
+        <v>-0.047303806990385056</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0.1843409687280655</v>
+        <v>0.017990050837397575</v>
       </c>
       <c r="B39" t="n">
-        <v>-0.04290863126516342</v>
+        <v>-0.10630770772695541</v>
       </c>
       <c r="C39" t="n">
-        <v>-0.1515471190214157</v>
+        <v>0.18209370970726013</v>
       </c>
       <c r="D39" t="n">
-        <v>-0.11306782066822052</v>
+        <v>-0.1183210164308548</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>-0.06841924041509628</v>
+        <v>-0.0028428654186427593</v>
       </c>
       <c r="B40" t="n">
-        <v>-0.03448006510734558</v>
+        <v>0.017564337700605392</v>
       </c>
       <c r="C40" t="n">
-        <v>-0.032103508710861206</v>
+        <v>-0.1792486310005188</v>
       </c>
       <c r="D40" t="n">
-        <v>0.2576909065246582</v>
+        <v>0.001828639768064022</v>
       </c>
     </row>
   </sheetData>
@@ -1212,562 +1212,562 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-0.07234886288642883</v>
+        <v>-0.06389649957418442</v>
       </c>
       <c r="B1" t="n">
-        <v>0.016882319003343582</v>
+        <v>-0.09124380350112915</v>
       </c>
       <c r="C1" t="n">
-        <v>0.016849800944328308</v>
+        <v>-0.004145781509578228</v>
       </c>
       <c r="D1" t="n">
-        <v>0.07007962465286255</v>
+        <v>-0.2186027467250824</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.03027351200580597</v>
+        <v>0.008080754429101944</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.05602988228201866</v>
+        <v>7.906928658485413E-6</v>
       </c>
       <c r="C2" t="n">
-        <v>0.04358048737049103</v>
+        <v>-0.0015023541636765003</v>
       </c>
       <c r="D2" t="n">
-        <v>0.062444254755973816</v>
+        <v>0.02818869799375534</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-0.09252998232841492</v>
+        <v>0.13749265670776367</v>
       </c>
       <c r="B3" t="n">
-        <v>0.03572581708431244</v>
+        <v>0.09560421109199524</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.12015296518802643</v>
+        <v>-0.01187186874449253</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2512970268726349</v>
+        <v>-0.06086069718003273</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.21395321190357208</v>
+        <v>0.04874947667121887</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.12084676325321198</v>
+        <v>-0.0274493470788002</v>
       </c>
       <c r="C4" t="n">
-        <v>0.011845389381051064</v>
+        <v>-0.05297337844967842</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.011316025629639626</v>
+        <v>0.1296500265598297</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.11970394104719162</v>
+        <v>-0.037702303379774094</v>
       </c>
       <c r="B5" t="n">
-        <v>0.1028914600610733</v>
+        <v>0.27591273188591003</v>
       </c>
       <c r="C5" t="n">
-        <v>0.16607482731342316</v>
+        <v>-0.00362224830314517</v>
       </c>
       <c r="D5" t="n">
-        <v>0.14305561780929565</v>
+        <v>-0.031522832810878754</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.15668773651123047</v>
+        <v>-0.055459361523389816</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.17120011150836945</v>
+        <v>-0.12109538167715073</v>
       </c>
       <c r="C6" t="n">
-        <v>0.18009509146213531</v>
+        <v>0.1620221585035324</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.10621798038482666</v>
+        <v>0.09444412589073181</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.24369460344314575</v>
+        <v>0.07399091124534607</v>
       </c>
       <c r="B7" t="n">
-        <v>0.28211498260498047</v>
+        <v>0.047157980501651764</v>
       </c>
       <c r="C7" t="n">
-        <v>0.019860174506902695</v>
+        <v>-0.13552571833133698</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0022366782650351524</v>
+        <v>-0.09829124063253403</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.09650485217571259</v>
+        <v>-0.037880945950746536</v>
       </c>
       <c r="B8" t="n">
-        <v>0.07375797629356384</v>
+        <v>0.055898718535900116</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.16692394018173218</v>
+        <v>0.03329382464289665</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.17126332223415375</v>
+        <v>0.15355098247528076</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.0028779571875929832</v>
+        <v>-0.02246752195060253</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.1883925199508667</v>
+        <v>-0.03677751123905182</v>
       </c>
       <c r="C9" t="n">
-        <v>0.008306041359901428</v>
+        <v>0.03611847013235092</v>
       </c>
       <c r="D9" t="n">
-        <v>0.1758582592010498</v>
+        <v>0.03136863186955452</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-0.09698314964771271</v>
+        <v>0.0642903745174408</v>
       </c>
       <c r="B10" t="n">
-        <v>0.0768687054514885</v>
+        <v>0.030198033899068832</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.09595997631549835</v>
+        <v>-0.1094447672367096</v>
       </c>
       <c r="D10" t="n">
-        <v>0.06529839336872101</v>
+        <v>-0.14488685131072998</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.024225160479545593</v>
+        <v>-0.3079129755496979</v>
       </c>
       <c r="B11" t="n">
-        <v>0.09643029421567917</v>
+        <v>0.06913980096578598</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.22879864275455475</v>
+        <v>0.011920605786144733</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.0523659884929657</v>
+        <v>0.2208564579486847</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.05337713658809662</v>
+        <v>-0.07692365348339081</v>
       </c>
       <c r="B12" t="n">
-        <v>0.20273429155349731</v>
+        <v>-0.07407177984714508</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0010745218023657799</v>
+        <v>-0.019008511677384377</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.04763869568705559</v>
+        <v>-0.007348686456680298</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.19907636940479279</v>
+        <v>0.05051497370004654</v>
       </c>
       <c r="B13" t="n">
-        <v>0.09057705849409103</v>
+        <v>-0.0423109196126461</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.057706836611032486</v>
+        <v>-0.013544466346502304</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.023008383810520172</v>
+        <v>0.2124316692352295</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.2157144397497177</v>
+        <v>-0.051885541528463364</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.04155682772397995</v>
+        <v>0.07659047842025757</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.07814832031726837</v>
+        <v>-0.008340846747159958</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.17448866367340088</v>
+        <v>-0.28722548484802246</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>-0.16252058744430542</v>
+        <v>-0.01754279062151909</v>
       </c>
       <c r="B15" t="n">
-        <v>0.152814120054245</v>
+        <v>0.042368434369564056</v>
       </c>
       <c r="C15" t="n">
-        <v>0.07722285389900208</v>
+        <v>0.03303954377770424</v>
       </c>
       <c r="D15" t="n">
-        <v>0.00682438537478447</v>
+        <v>-0.03768201917409897</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.052035048604011536</v>
+        <v>0.009749118238687515</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.04871005937457085</v>
+        <v>0.05711869150400162</v>
       </c>
       <c r="C16" t="n">
-        <v>0.004592357203364372</v>
+        <v>0.1435820758342743</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.04693888872861862</v>
+        <v>0.07921159267425537</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>-0.21952836215496063</v>
+        <v>-0.17263871431350708</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.004837876185774803</v>
+        <v>0.009999902918934822</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.0392114631831646</v>
+        <v>-0.13049989938735962</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.12442920356988907</v>
+        <v>0.03834359347820282</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.07061295211315155</v>
+        <v>-0.005634240806102753</v>
       </c>
       <c r="B18" t="n">
-        <v>0.0745324194431305</v>
+        <v>-0.03521981090307236</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.08626613765954971</v>
+        <v>-0.19998985528945923</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.2479885220527649</v>
+        <v>-0.14725403487682343</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>-0.00694509781897068</v>
+        <v>0.019050732254981995</v>
       </c>
       <c r="B19" t="n">
-        <v>0.24852365255355835</v>
+        <v>0.02046559378504753</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.06290069222450256</v>
+        <v>-0.09790496528148651</v>
       </c>
       <c r="D19" t="n">
-        <v>0.037260521203279495</v>
+        <v>0.15286219120025635</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.05615841597318649</v>
+        <v>-0.028479762375354767</v>
       </c>
       <c r="B20" t="n">
-        <v>0.03054730035364628</v>
+        <v>-0.09414160996675491</v>
       </c>
       <c r="C20" t="n">
-        <v>0.014693856239318848</v>
+        <v>-0.07840527594089508</v>
       </c>
       <c r="D20" t="n">
-        <v>0.012059947475790977</v>
+        <v>-0.052012849599123</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>-0.20210000872612</v>
+        <v>-0.17854121327400208</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.007044300436973572</v>
+        <v>0.024987762793898582</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.03357400372624397</v>
+        <v>-7.69222155213356E-4</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.008465394377708435</v>
+        <v>-0.07213828712701797</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.05419458448886871</v>
+        <v>-0.011184588074684143</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.018324943259358406</v>
+        <v>-0.004326232708990574</v>
       </c>
       <c r="C22" t="n">
-        <v>0.14954787492752075</v>
+        <v>0.06411624699831009</v>
       </c>
       <c r="D22" t="n">
-        <v>0.040239620953798294</v>
+        <v>-0.03204920142889023</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.03145187720656395</v>
+        <v>0.06649229675531387</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.010178670287132263</v>
+        <v>-0.06789644807577133</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.10887745022773743</v>
+        <v>0.07078349590301514</v>
       </c>
       <c r="D23" t="n">
-        <v>0.0013189841993153095</v>
+        <v>-0.039708156138658524</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.020300090312957764</v>
+        <v>0.031162884086370468</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.06181376427412033</v>
+        <v>0.10898064821958542</v>
       </c>
       <c r="C24" t="n">
-        <v>0.12536850571632385</v>
+        <v>-0.06939622759819031</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.11869697272777557</v>
+        <v>-0.02359776571393013</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>-0.47354644536972046</v>
+        <v>-0.047447796911001205</v>
       </c>
       <c r="B25" t="n">
-        <v>0.06096680462360382</v>
+        <v>0.05096514895558357</v>
       </c>
       <c r="C25" t="n">
-        <v>0.10411477088928223</v>
+        <v>0.12400415539741516</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.015085866674780846</v>
+        <v>-0.08187992870807648</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>-0.026893600821495056</v>
+        <v>0.04946713149547577</v>
       </c>
       <c r="B26" t="n">
-        <v>-0.10543301701545715</v>
+        <v>0.015651986002922058</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.07219544798135757</v>
+        <v>-0.014398708008229733</v>
       </c>
       <c r="D26" t="n">
-        <v>0.10725624859333038</v>
+        <v>0.02091211825609207</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>-0.09445516765117645</v>
+        <v>-0.033368464559316635</v>
       </c>
       <c r="B27" t="n">
-        <v>0.10327683389186859</v>
+        <v>-0.0729263499379158</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.05561073124408722</v>
+        <v>-0.05274062976241112</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.031994253396987915</v>
+        <v>-0.0538196824491024</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.05188238248229027</v>
+        <v>0.0536486953496933</v>
       </c>
       <c r="B28" t="n">
-        <v>0.2559647262096405</v>
+        <v>0.011592373251914978</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.05699727684259415</v>
+        <v>-0.009315858595073223</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.04165206849575043</v>
+        <v>-0.057237572968006134</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>-0.2679425776004791</v>
+        <v>0.07360254973173141</v>
       </c>
       <c r="B29" t="n">
-        <v>0.16579388082027435</v>
+        <v>0.01676642708480358</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.15592531859874725</v>
+        <v>-0.028576508164405823</v>
       </c>
       <c r="D29" t="n">
-        <v>-0.09141124039888382</v>
+        <v>0.052261561155319214</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>-0.21645116806030273</v>
+        <v>0.0744008868932724</v>
       </c>
       <c r="B30" t="n">
-        <v>0.10617121309041977</v>
+        <v>0.055456407368183136</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.020537223666906357</v>
+        <v>-0.041889261454343796</v>
       </c>
       <c r="D30" t="n">
-        <v>0.05493501201272011</v>
+        <v>0.11539063602685928</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.04057598114013672</v>
+        <v>-0.09239716082811356</v>
       </c>
       <c r="B31" t="n">
-        <v>0.1943371295928955</v>
+        <v>-0.06696857511997223</v>
       </c>
       <c r="C31" t="n">
-        <v>-0.058336712419986725</v>
+        <v>-0.026088804006576538</v>
       </c>
       <c r="D31" t="n">
-        <v>0.11391328275203705</v>
+        <v>0.15469320118427277</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>-0.058815427124500275</v>
+        <v>-0.021047579124569893</v>
       </c>
       <c r="B32" t="n">
-        <v>-0.012685430236160755</v>
+        <v>-0.06431180238723755</v>
       </c>
       <c r="C32" t="n">
-        <v>0.06164507567882538</v>
+        <v>0.033154167234897614</v>
       </c>
       <c r="D32" t="n">
-        <v>0.012881647795438766</v>
+        <v>-2.843700349330902E-4</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>-0.01334843784570694</v>
+        <v>0.0577424056828022</v>
       </c>
       <c r="B33" t="n">
-        <v>-0.060623809695243835</v>
+        <v>-0.1274203211069107</v>
       </c>
       <c r="C33" t="n">
-        <v>0.013025723397731781</v>
+        <v>0.053209058940410614</v>
       </c>
       <c r="D33" t="n">
-        <v>0.048185937106609344</v>
+        <v>-0.04601828753948212</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0.017271552234888077</v>
+        <v>-0.032432086765766144</v>
       </c>
       <c r="B34" t="n">
-        <v>0.009487006813287735</v>
+        <v>-0.029296452179551125</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.009161055088043213</v>
+        <v>-0.09495723247528076</v>
       </c>
       <c r="D34" t="n">
-        <v>0.11633709073066711</v>
+        <v>-0.02454639971256256</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0.13111388683319092</v>
+        <v>0.05811196193099022</v>
       </c>
       <c r="B35" t="n">
-        <v>0.10975617170333862</v>
+        <v>-0.0453496091067791</v>
       </c>
       <c r="C35" t="n">
-        <v>0.20306268334388733</v>
+        <v>0.044381022453308105</v>
       </c>
       <c r="D35" t="n">
-        <v>0.09213129431009293</v>
+        <v>-0.04849528148770332</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0.2040126919746399</v>
+        <v>-0.2414308488368988</v>
       </c>
       <c r="B36" t="n">
-        <v>-0.05980166420340538</v>
+        <v>0.060495615005493164</v>
       </c>
       <c r="C36" t="n">
-        <v>0.06966003775596619</v>
+        <v>-0.15227888524532318</v>
       </c>
       <c r="D36" t="n">
-        <v>-0.024399885907769203</v>
+        <v>0.060439273715019226</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0.06089802831411362</v>
+        <v>0.025792095810174942</v>
       </c>
       <c r="B37" t="n">
-        <v>-0.11898385733366013</v>
+        <v>-0.06560743600130081</v>
       </c>
       <c r="C37" t="n">
-        <v>-0.0059860944747924805</v>
+        <v>0.06886830925941467</v>
       </c>
       <c r="D37" t="n">
-        <v>0.1128484457731247</v>
+        <v>-0.008360255509614944</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0.20190726220607758</v>
+        <v>-0.023360799998044968</v>
       </c>
       <c r="B38" t="n">
-        <v>0.03724940866231918</v>
+        <v>0.045467618852853775</v>
       </c>
       <c r="C38" t="n">
-        <v>-0.17258267104625702</v>
+        <v>-3.106929361820221E-4</v>
       </c>
       <c r="D38" t="n">
-        <v>0.024375908076763153</v>
+        <v>0.13138476014137268</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0.05027315020561218</v>
+        <v>0.03193189948797226</v>
       </c>
       <c r="B39" t="n">
-        <v>-0.029163772240281105</v>
+        <v>0.19669821858406067</v>
       </c>
       <c r="C39" t="n">
-        <v>0.1049346774816513</v>
+        <v>-0.007279247045516968</v>
       </c>
       <c r="D39" t="n">
-        <v>0.1246844157576561</v>
+        <v>-0.10375549644231796</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>-0.1902463436126709</v>
+        <v>-8.456073701381683E-4</v>
       </c>
       <c r="B40" t="n">
-        <v>0.018578846007585526</v>
+        <v>-0.12867090106010437</v>
       </c>
       <c r="C40" t="n">
-        <v>0.3138689398765564</v>
+        <v>-0.02254832722246647</v>
       </c>
       <c r="D40" t="n">
-        <v>0.02998977340757847</v>
+        <v>-0.03866763040423393</v>
       </c>
     </row>
   </sheetData>
@@ -1785,562 +1785,562 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.13992388546466827</v>
+        <v>0.10933744162321091</v>
       </c>
       <c r="B1" t="n">
-        <v>-0.16180171072483063</v>
+        <v>0.014019832015037537</v>
       </c>
       <c r="C1" t="n">
-        <v>0.02662740647792816</v>
+        <v>-0.018004152923822403</v>
       </c>
       <c r="D1" t="n">
-        <v>-0.26991167664527893</v>
+        <v>-0.152528315782547</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.018953237682580948</v>
+        <v>-0.11643366515636444</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.039441436529159546</v>
+        <v>-0.1187732070684433</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.09714987128973007</v>
+        <v>-0.13103635609149933</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.08368244022130966</v>
+        <v>0.050826359540224075</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-0.05840936303138733</v>
+        <v>-0.11383438110351562</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.06974527984857559</v>
+        <v>0.011949293315410614</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.02720548026263714</v>
+        <v>-0.06698615103960037</v>
       </c>
       <c r="D3" t="n">
-        <v>0.030907876789569855</v>
+        <v>0.09473228454589844</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.008097108453512192</v>
+        <v>-0.03715265914797783</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.042607396841049194</v>
+        <v>0.009414367377758026</v>
       </c>
       <c r="C4" t="n">
-        <v>0.048238106071949005</v>
+        <v>-0.006599975284188986</v>
       </c>
       <c r="D4" t="n">
-        <v>0.39232248067855835</v>
+        <v>-0.10752151906490326</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.0013126526027917862</v>
+        <v>-0.05375484749674797</v>
       </c>
       <c r="B5" t="n">
-        <v>0.043589040637016296</v>
+        <v>-0.010021472349762917</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.006839044392108917</v>
+        <v>-0.02148427814245224</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.01787285879254341</v>
+        <v>0.05570046976208687</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.09270893037319183</v>
+        <v>7.571689784526825E-4</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.1725033074617386</v>
+        <v>-0.03258749470114708</v>
       </c>
       <c r="C6" t="n">
-        <v>0.07689066976308823</v>
+        <v>0.016790788620710373</v>
       </c>
       <c r="D6" t="n">
-        <v>0.15492558479309082</v>
+        <v>0.02973402664065361</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-0.005527548957616091</v>
+        <v>-0.10314793884754181</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.04495228826999664</v>
+        <v>0.0023990999907255173</v>
       </c>
       <c r="C7" t="n">
-        <v>0.15550418198108673</v>
+        <v>0.1342679113149643</v>
       </c>
       <c r="D7" t="n">
-        <v>0.05945468321442604</v>
+        <v>0.011989607475697994</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.04694207012653351</v>
+        <v>0.12069403380155563</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.04585389792919159</v>
+        <v>0.02316521853208542</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.21417108178138733</v>
+        <v>-0.1414446383714676</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.16197852790355682</v>
+        <v>-0.08602568507194519</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.08873778581619263</v>
+        <v>-0.0899713858962059</v>
       </c>
       <c r="B9" t="n">
-        <v>0.03091985546052456</v>
+        <v>-0.21015185117721558</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.010180477984249592</v>
+        <v>0.05723162740468979</v>
       </c>
       <c r="D9" t="n">
-        <v>0.04002000391483307</v>
+        <v>-0.0793183296918869</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.09173401445150375</v>
+        <v>0.005559735931456089</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.13036683201789856</v>
+        <v>0.09251393377780914</v>
       </c>
       <c r="C10" t="n">
-        <v>0.08912487328052521</v>
+        <v>-0.17307338118553162</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1764889806509018</v>
+        <v>0.08166040480136871</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>-0.0375543013215065</v>
+        <v>-0.11398792266845703</v>
       </c>
       <c r="B11" t="n">
-        <v>0.009475421160459518</v>
+        <v>-0.22430169582366943</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.13423112034797668</v>
+        <v>0.03703782707452774</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.002667137421667576</v>
+        <v>-0.09721887111663818</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.36446714401245117</v>
+        <v>-0.04463692009449005</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.040558211505413055</v>
+        <v>0.11199672520160675</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.011160895228385925</v>
+        <v>0.09206048399209976</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.06950130313634872</v>
+        <v>0.0659489557147026</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>-0.06230617314577103</v>
+        <v>0.1660011261701584</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.07733767479658127</v>
+        <v>0.010774888098239899</v>
       </c>
       <c r="C13" t="n">
-        <v>0.12711763381958008</v>
+        <v>0.011974839493632317</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.05629507452249527</v>
+        <v>0.020712733268737793</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.1519984006881714</v>
+        <v>-0.034100327640771866</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.015934094786643982</v>
+        <v>0.010783635079860687</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.024987241253256798</v>
+        <v>-0.08582564443349838</v>
       </c>
       <c r="D14" t="n">
-        <v>0.03978830948472023</v>
+        <v>-0.050364114344120026</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.08925891667604446</v>
+        <v>-0.10022668540477753</v>
       </c>
       <c r="B15" t="n">
-        <v>0.07645067572593689</v>
+        <v>0.025943897664546967</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.004094228148460388</v>
+        <v>0.09310247004032135</v>
       </c>
       <c r="D15" t="n">
-        <v>0.28474417328834534</v>
+        <v>0.03284043073654175</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>-0.15745143592357635</v>
+        <v>0.08469495177268982</v>
       </c>
       <c r="B16" t="n">
-        <v>0.05537768080830574</v>
+        <v>-0.08095400780439377</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.009224623441696167</v>
+        <v>0.10704676806926727</v>
       </c>
       <c r="D16" t="n">
-        <v>0.1308169662952423</v>
+        <v>0.07937925308942795</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.12229884415864944</v>
+        <v>-0.022965148091316223</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.04716390743851662</v>
+        <v>-0.11477680504322052</v>
       </c>
       <c r="C17" t="n">
-        <v>0.08455482125282288</v>
+        <v>-0.1222759485244751</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0690678283572197</v>
+        <v>-0.06856109201908112</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>-0.02591853030025959</v>
+        <v>-0.03076452761888504</v>
       </c>
       <c r="B18" t="n">
-        <v>0.03972308337688446</v>
+        <v>-0.10624907910823822</v>
       </c>
       <c r="C18" t="n">
-        <v>0.01596910133957863</v>
+        <v>0.002319168299436569</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.04384813457727432</v>
+        <v>0.08722835034132004</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.047573983669281006</v>
+        <v>-0.11425339430570602</v>
       </c>
       <c r="B19" t="n">
-        <v>0.03550684079527855</v>
+        <v>0.16446462273597717</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.16159655153751373</v>
+        <v>-0.21856826543807983</v>
       </c>
       <c r="D19" t="n">
-        <v>0.07109849900007248</v>
+        <v>-0.09021097421646118</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>-0.2261521965265274</v>
+        <v>-6.746500730514526E-4</v>
       </c>
       <c r="B20" t="n">
-        <v>0.10292544960975647</v>
+        <v>-0.10031695663928986</v>
       </c>
       <c r="C20" t="n">
-        <v>0.07675379514694214</v>
+        <v>0.07530692964792252</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.03463767468929291</v>
+        <v>-0.1363891065120697</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>-0.09599070250988007</v>
+        <v>-0.15406323969364166</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.10416705161333084</v>
+        <v>-0.1469244509935379</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.037860382348299026</v>
+        <v>0.008759066462516785</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.023749705404043198</v>
+        <v>0.003549821674823761</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.09728679060935974</v>
+        <v>0.02924184873700142</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.10535600036382675</v>
+        <v>-0.1617705374956131</v>
       </c>
       <c r="C22" t="n">
-        <v>0.10668451339006424</v>
+        <v>-0.3831351399421692</v>
       </c>
       <c r="D22" t="n">
-        <v>-0.006875615566968918</v>
+        <v>-0.03251313790678978</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.06838533282279968</v>
+        <v>0.10465993732213974</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.09795000404119492</v>
+        <v>0.14006862044334412</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.15300627052783966</v>
+        <v>-0.04304962232708931</v>
       </c>
       <c r="D23" t="n">
-        <v>0.04376912862062454</v>
+        <v>0.13710777461528778</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.01673227921128273</v>
+        <v>0.22715546190738678</v>
       </c>
       <c r="B24" t="n">
-        <v>0.14271323382854462</v>
+        <v>-0.08880610764026642</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.1858443319797516</v>
+        <v>0.05496445298194885</v>
       </c>
       <c r="D24" t="n">
-        <v>0.04502486437559128</v>
+        <v>0.1111479103565216</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.0201391763985157</v>
+        <v>0.03502148017287254</v>
       </c>
       <c r="B25" t="n">
-        <v>0.18042433261871338</v>
+        <v>0.06238193437457085</v>
       </c>
       <c r="C25" t="n">
-        <v>0.12238913029432297</v>
+        <v>-0.0032640895806252956</v>
       </c>
       <c r="D25" t="n">
-        <v>0.11050635576248169</v>
+        <v>0.10302641242742538</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>-0.3347679376602173</v>
+        <v>-0.0847831666469574</v>
       </c>
       <c r="B26" t="n">
-        <v>0.1851436197757721</v>
+        <v>-0.09622442722320557</v>
       </c>
       <c r="C26" t="n">
-        <v>0.09950220584869385</v>
+        <v>0.06272101402282715</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.006356316152960062</v>
+        <v>-0.07335658371448517</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>-0.0063226306810975075</v>
+        <v>0.08545935153961182</v>
       </c>
       <c r="B27" t="n">
-        <v>0.2622978091239929</v>
+        <v>0.0169889684766531</v>
       </c>
       <c r="C27" t="n">
-        <v>0.11814422160387039</v>
+        <v>-0.057116203010082245</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.009072443470358849</v>
+        <v>-0.0670105516910553</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.22076769173145294</v>
+        <v>0.07086454331874847</v>
       </c>
       <c r="B28" t="n">
-        <v>0.054100073873996735</v>
+        <v>0.005778050050139427</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.10277161747217178</v>
+        <v>0.0064976029098033905</v>
       </c>
       <c r="D28" t="n">
-        <v>0.15757881104946136</v>
+        <v>0.03351236507296562</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>-0.05108040198683739</v>
+        <v>0.08641329407691956</v>
       </c>
       <c r="B29" t="n">
-        <v>-0.06569618731737137</v>
+        <v>-0.11831073462963104</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.03532780334353447</v>
+        <v>-0.0345211960375309</v>
       </c>
       <c r="D29" t="n">
-        <v>-0.00920521467924118</v>
+        <v>-0.034599870443344116</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.04218510910868645</v>
+        <v>0.030198022723197937</v>
       </c>
       <c r="B30" t="n">
-        <v>-0.032286033034324646</v>
+        <v>0.038798004388809204</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.10695703327655792</v>
+        <v>0.05006437003612518</v>
       </c>
       <c r="D30" t="n">
-        <v>0.15717653930187225</v>
+        <v>0.0417705774307251</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.03129013255238533</v>
+        <v>-0.05164986103773117</v>
       </c>
       <c r="B31" t="n">
-        <v>0.09252665936946869</v>
+        <v>0.01597405970096588</v>
       </c>
       <c r="C31" t="n">
-        <v>0.03835779428482056</v>
+        <v>-0.027267633005976677</v>
       </c>
       <c r="D31" t="n">
-        <v>0.04557880014181137</v>
+        <v>-0.06550753861665726</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>-0.07094521820545197</v>
+        <v>0.05225735902786255</v>
       </c>
       <c r="B32" t="n">
-        <v>0.022167213261127472</v>
+        <v>-0.18249452114105225</v>
       </c>
       <c r="C32" t="n">
-        <v>-0.02126605249941349</v>
+        <v>0.08252683281898499</v>
       </c>
       <c r="D32" t="n">
-        <v>-0.18901142477989197</v>
+        <v>0.057334307581186295</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0.03456640988588333</v>
+        <v>0.14036083221435547</v>
       </c>
       <c r="B33" t="n">
-        <v>-0.34340161085128784</v>
+        <v>0.0906350165605545</v>
       </c>
       <c r="C33" t="n">
-        <v>0.10864310711622238</v>
+        <v>0.0457361564040184</v>
       </c>
       <c r="D33" t="n">
-        <v>0.02738972380757332</v>
+        <v>-0.01037389412522316</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0.05759868398308754</v>
+        <v>-0.05068881809711456</v>
       </c>
       <c r="B34" t="n">
-        <v>0.041134998202323914</v>
+        <v>-0.24826696515083313</v>
       </c>
       <c r="C34" t="n">
-        <v>0.10609288513660431</v>
+        <v>-0.03498928248882294</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.0030384808778762817</v>
+        <v>0.041352517902851105</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0.010707147419452667</v>
+        <v>-0.033584609627723694</v>
       </c>
       <c r="B35" t="n">
-        <v>-0.08696112781763077</v>
+        <v>-0.046658940613269806</v>
       </c>
       <c r="C35" t="n">
-        <v>0.05836135149002075</v>
+        <v>0.002283269539475441</v>
       </c>
       <c r="D35" t="n">
-        <v>0.10217086970806122</v>
+        <v>0.04410167783498764</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0.01682087406516075</v>
+        <v>-0.059356868267059326</v>
       </c>
       <c r="B36" t="n">
-        <v>-0.09764131903648376</v>
+        <v>0.20265823602676392</v>
       </c>
       <c r="C36" t="n">
-        <v>0.029623929411172867</v>
+        <v>-0.0593113973736763</v>
       </c>
       <c r="D36" t="n">
-        <v>-0.06982618570327759</v>
+        <v>-0.04936816543340683</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>-0.05170474201440811</v>
+        <v>0.0374433659017086</v>
       </c>
       <c r="B37" t="n">
-        <v>0.03287079930305481</v>
+        <v>0.021484918892383575</v>
       </c>
       <c r="C37" t="n">
-        <v>-0.0382121205329895</v>
+        <v>-0.16000255942344666</v>
       </c>
       <c r="D37" t="n">
-        <v>-0.04709576815366745</v>
+        <v>-0.08149866759777069</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>-0.14386224746704102</v>
+        <v>0.06822774559259415</v>
       </c>
       <c r="B38" t="n">
-        <v>-0.061433494091033936</v>
+        <v>-0.049574293196201324</v>
       </c>
       <c r="C38" t="n">
-        <v>-0.07773032784461975</v>
+        <v>0.053040534257888794</v>
       </c>
       <c r="D38" t="n">
-        <v>-0.1516622006893158</v>
+        <v>-0.06316842138767242</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>-0.019100677222013474</v>
+        <v>0.0721774622797966</v>
       </c>
       <c r="B39" t="n">
-        <v>-0.045530740171670914</v>
+        <v>-0.011005617678165436</v>
       </c>
       <c r="C39" t="n">
-        <v>0.037922561168670654</v>
+        <v>-0.01628868654370308</v>
       </c>
       <c r="D39" t="n">
-        <v>0.029690178111195564</v>
+        <v>0.08997579663991928</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0.2330261617898941</v>
+        <v>0.0021876292303204536</v>
       </c>
       <c r="B40" t="n">
-        <v>-0.020425736904144287</v>
+        <v>0.025890033692121506</v>
       </c>
       <c r="C40" t="n">
-        <v>0.10207906365394592</v>
+        <v>-0.1578218936920166</v>
       </c>
       <c r="D40" t="n">
-        <v>0.08011676371097565</v>
+        <v>-0.04593376815319061</v>
       </c>
     </row>
   </sheetData>

</xml_diff>